<commit_message>
adding all edits to edition 5
</commit_message>
<xml_diff>
--- a/data/WHO_Tumors/intermediate/df_5th_edition_manual_edit.xlsx
+++ b/data/WHO_Tumors/intermediate/df_5th_edition_manual_edit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lahiria/Desktop/MTP_Paper/CT-Embedding-Paper/data/WHO_Tumors/intermediate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{723D31AB-168A-7445-864C-56DDAE35B8B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D1B6DA-453F-F740-9FF2-240D144DAEFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-3120" windowWidth="38400" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10808" uniqueCount="2878">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10843" uniqueCount="3059">
   <si>
     <t>Tumor_Names</t>
   </si>
@@ -8656,6 +8656,549 @@
   </si>
   <si>
     <t>neuroepithelial tumours</t>
+  </si>
+  <si>
+    <t>secondary cutaneous involvement in t-cell and nk-cell lymphomas</t>
+  </si>
+  <si>
+    <t>secondary cutaneous involvement in t-cell and nk-cell leukaemias</t>
+  </si>
+  <si>
+    <t>secondary cutaneous involvement in t-cell lymphomas and leukaemias</t>
+  </si>
+  <si>
+    <t>secondary cutaneous involvement in nk-cell lymphomas and leukaemias</t>
+  </si>
+  <si>
+    <t>secondary cutaneous involvement in t-cell lymphomas</t>
+  </si>
+  <si>
+    <t>secondary cutaneous involvement in nk-cell lymphomas</t>
+  </si>
+  <si>
+    <t>secondary cutaneous involvement in t-cell leukaemias</t>
+  </si>
+  <si>
+    <t>secondary cutaneous involvement in nk-cell leukaemias</t>
+  </si>
+  <si>
+    <t xml:space="preserve">seromucinous cystadenoma </t>
+  </si>
+  <si>
+    <t>seromucinous adenofibroma</t>
+  </si>
+  <si>
+    <t>serotonin-producing tumours with carcinoid syndrome</t>
+  </si>
+  <si>
+    <t>serotonin-producing tumours without carcinoid syndrome</t>
+  </si>
+  <si>
+    <t>serous adenofibroma of the fallopian tube</t>
+  </si>
+  <si>
+    <t>serous papilloma of the fallopian tube</t>
+  </si>
+  <si>
+    <t>other tumours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">simple lentigo </t>
+  </si>
+  <si>
+    <t>lentiginous melanocytic naevus</t>
+  </si>
+  <si>
+    <t>small intestinal neuroendocrine neoplasms</t>
+  </si>
+  <si>
+    <t>ampullary neuroendocrine neoplasms</t>
+  </si>
+  <si>
+    <t>solid papillary carcinoma (in situ)</t>
+  </si>
+  <si>
+    <t>solid papillary carcinoma (invasive)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spindle cell lipoma </t>
+  </si>
+  <si>
+    <t>splenic b-cell lymphomas</t>
+  </si>
+  <si>
+    <t>splenic b-cell leukaemias</t>
+  </si>
+  <si>
+    <t>squamous dysplasia of the lung</t>
+  </si>
+  <si>
+    <t>carcinoma in situ of the lung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">squamous papilloma </t>
+  </si>
+  <si>
+    <t>squamous papillomatosis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stromal hyperplasia </t>
+  </si>
+  <si>
+    <t>stromal hyperthecosis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t-cell and nk-cell lymphoid proliferations </t>
+  </si>
+  <si>
+    <t xml:space="preserve">t-cell lymphoid proliferations </t>
+  </si>
+  <si>
+    <t xml:space="preserve">nk-cell lymphoid proliferations </t>
+  </si>
+  <si>
+    <t>t-cell and nk-cell lymphomas</t>
+  </si>
+  <si>
+    <t>nk-cell lymphomas</t>
+  </si>
+  <si>
+    <t>t-cell lymphoid proliferations and lymphomas</t>
+  </si>
+  <si>
+    <t>nk-cell lymphoid proliferations and lymphomas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">trichodiscomas </t>
+  </si>
+  <si>
+    <t>fibrofolliculomas</t>
+  </si>
+  <si>
+    <t>tufted angioma</t>
+  </si>
+  <si>
+    <t>kaposiform haemangioendothelioma</t>
+  </si>
+  <si>
+    <t>tumour-like lesions of the conjunctiva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tumours and tumour-like lesions of the neck </t>
+  </si>
+  <si>
+    <t>tumours and tumour-like lesions of the lymph nodes</t>
+  </si>
+  <si>
+    <t>tumours of the neck and lymph nodes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tumours of the neck </t>
+  </si>
+  <si>
+    <t>tumours of the lymph nodes</t>
+  </si>
+  <si>
+    <t>tumour-like lesions of the neck and lymph nodes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tumour-like lesions of the neck </t>
+  </si>
+  <si>
+    <t>tumour-like lesions of the lymph nodes</t>
+  </si>
+  <si>
+    <t>tumours of haematopoietic origin</t>
+  </si>
+  <si>
+    <t>tumours of lymphoid origin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tumours of the adrenal medulla </t>
+  </si>
+  <si>
+    <t>tumours of the extra-adrenal paraganglia</t>
+  </si>
+  <si>
+    <t>tumours of the broad ligament</t>
+  </si>
+  <si>
+    <t>tumours of other uterine ligaments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tumours of the collecting ducts </t>
+  </si>
+  <si>
+    <t>tumours of the rete testis</t>
+  </si>
+  <si>
+    <t>tumours of the colon</t>
+  </si>
+  <si>
+    <t>tumours of the rectum</t>
+  </si>
+  <si>
+    <t>tumours of the conjunctiva</t>
+  </si>
+  <si>
+    <t>tumours of the caruncle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tumours of the gallbladder </t>
+  </si>
+  <si>
+    <t>tumours of the extrahepatic bile ducts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tumours of the iris </t>
+  </si>
+  <si>
+    <t>tumours of the ciliary body neuroepithelium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tumours of the liver </t>
+  </si>
+  <si>
+    <t>tumours of the intrahepatic bile ducts</t>
+  </si>
+  <si>
+    <t>tumours of the middle ear</t>
+  </si>
+  <si>
+    <t>tumours of the inner ear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tumours of the optic disc </t>
+  </si>
+  <si>
+    <t>tumours of the optic nerve</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tumours of the penis </t>
+  </si>
+  <si>
+    <t>tumours of the scrotum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tumours of the pleura </t>
+  </si>
+  <si>
+    <t>tumours of the pericardium</t>
+  </si>
+  <si>
+    <t>tumours of the retina</t>
+  </si>
+  <si>
+    <t>tumours of the neuroepithelium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tumours of the small intestine </t>
+  </si>
+  <si>
+    <t>tumours of the ampulla</t>
+  </si>
+  <si>
+    <t>tumours with apocrine differentiation</t>
+  </si>
+  <si>
+    <t>tumours with eccrine differentiation</t>
+  </si>
+  <si>
+    <t>undifferentiated carcinomas of the ovary</t>
+  </si>
+  <si>
+    <t>dedifferentiated carcinomas of the ovary</t>
+  </si>
+  <si>
+    <t>undifferentiated carcinomas of the uterine corpus</t>
+  </si>
+  <si>
+    <t>dedifferentiated carcinomas of the uterine corpus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">undifferentiated small round cell sarcomas of bone </t>
+  </si>
+  <si>
+    <t>undifferentiated small round cell sarcomas of soft tissue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">undifferentiated small round cell sarcomas of soft tissue </t>
+  </si>
+  <si>
+    <t>undifferentiated small round cell sarcomas of bone</t>
+  </si>
+  <si>
+    <t>urachal neoplasms</t>
+  </si>
+  <si>
+    <t>diverticular neoplasms</t>
+  </si>
+  <si>
+    <t>urinary tumours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verruca plantaris </t>
+  </si>
+  <si>
+    <t>verruca palmaris</t>
+  </si>
+  <si>
+    <t>verrucous carcinoma of the oral cavity</t>
+  </si>
+  <si>
+    <t>verrucous carcinoma of the mobile tongue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wolffian tumour of the broad ligament </t>
+  </si>
+  <si>
+    <t>wolffian tumour of other uterine ligaments</t>
+  </si>
+  <si>
+    <t>bartholin gland hyperplasia</t>
+  </si>
+  <si>
+    <t>bartholin gland adenoma</t>
+  </si>
+  <si>
+    <t>bartholin gland adenomyoma</t>
+  </si>
+  <si>
+    <t>benign fibroblastic neoplasms</t>
+  </si>
+  <si>
+    <t>myofibroblastic neoplasms</t>
+  </si>
+  <si>
+    <t>fibrohistiocytic neoplasms</t>
+  </si>
+  <si>
+    <t>benign myofibroblastic neoplasms</t>
+  </si>
+  <si>
+    <t>benign fibrohistiocytic neoplasms</t>
+  </si>
+  <si>
+    <t>central chondrosarcoma, grades 2</t>
+  </si>
+  <si>
+    <t>central chondrosarcoma, grades 3</t>
+  </si>
+  <si>
+    <t>conjunctival junctional naevi</t>
+  </si>
+  <si>
+    <t>compound naevi</t>
+  </si>
+  <si>
+    <t>subepithelial naevi</t>
+  </si>
+  <si>
+    <t>fibrohistiocytic tumours</t>
+  </si>
+  <si>
+    <t>gliomas</t>
+  </si>
+  <si>
+    <t>hypopharyngeal tumours</t>
+  </si>
+  <si>
+    <t>laryngeal tumours</t>
+  </si>
+  <si>
+    <t>tracheal tumours</t>
+  </si>
+  <si>
+    <t>parapharyngeal tumours</t>
+  </si>
+  <si>
+    <t>intermediate fibroblastic neoplasms</t>
+  </si>
+  <si>
+    <t>intermediate myofibroblastic neoplasms</t>
+  </si>
+  <si>
+    <t>intermediate fibrohistiocytic neoplasms</t>
+  </si>
+  <si>
+    <t>subepithelial conjunctival naevi</t>
+  </si>
+  <si>
+    <t>junctional naevi</t>
+  </si>
+  <si>
+    <t>dermal naevi</t>
+  </si>
+  <si>
+    <t>malignant fibroblastic neoplasms</t>
+  </si>
+  <si>
+    <t>meningioma of the sinonasal tract</t>
+  </si>
+  <si>
+    <t>meningioma of the ear</t>
+  </si>
+  <si>
+    <t>meningioma of the temporal bone</t>
+  </si>
+  <si>
+    <t>mesenchymal tumours unique to the hypopharynx</t>
+  </si>
+  <si>
+    <t>mesenchymal tumours unique to the larynx</t>
+  </si>
+  <si>
+    <t>mesenchymal tumours unique to the trachea</t>
+  </si>
+  <si>
+    <t>mesenchymal tumours unique to the parapharyngeal space</t>
+  </si>
+  <si>
+    <t>mixed teratoma, prepubertal-type</t>
+  </si>
+  <si>
+    <t>nasal tumours</t>
+  </si>
+  <si>
+    <t>paranasal tumours</t>
+  </si>
+  <si>
+    <t>skull base tumours</t>
+  </si>
+  <si>
+    <t>nodular fasciitis, proliferative myositis</t>
+  </si>
+  <si>
+    <t>proliferative fasciitis, proliferative myositis</t>
+  </si>
+  <si>
+    <t>nodular and proliferative fasciitis</t>
+  </si>
+  <si>
+    <t>proliferative fasciitis</t>
+  </si>
+  <si>
+    <t>naevoid melanomas</t>
+  </si>
+  <si>
+    <t>pituicytoma</t>
+  </si>
+  <si>
+    <t>granular cell tumour of the sellar region</t>
+  </si>
+  <si>
+    <t>spindle cell oncocytoma</t>
+  </si>
+  <si>
+    <t>reactive lesions</t>
+  </si>
+  <si>
+    <t>epithelial lesions</t>
+  </si>
+  <si>
+    <t>degenerative conjunctival lesions</t>
+  </si>
+  <si>
+    <t>rete cystadenoma</t>
+  </si>
+  <si>
+    <t>rete adenoma</t>
+  </si>
+  <si>
+    <t>rete adenocarcinoma</t>
+  </si>
+  <si>
+    <t>sebaceous hyperplasia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">secondary peripheral chondrosarcoma, grades 2 </t>
+  </si>
+  <si>
+    <t>secondary peripheral chondrosarcoma, grades 3</t>
+  </si>
+  <si>
+    <t>serous cystadenoma of the ovary</t>
+  </si>
+  <si>
+    <t>serous adenofibroma of the ovary</t>
+  </si>
+  <si>
+    <t>serous surface papilloma of the ovary</t>
+  </si>
+  <si>
+    <t>special-site naevi (of the breast)</t>
+  </si>
+  <si>
+    <t>special-site naevi (of the axilla)</t>
+  </si>
+  <si>
+    <t>special-site naevi (of the scalp)</t>
+  </si>
+  <si>
+    <t>special-site naevi (of the ear)</t>
+  </si>
+  <si>
+    <t>teratomas</t>
+  </si>
+  <si>
+    <t>choristomas</t>
+  </si>
+  <si>
+    <t>tumour-like lesions of the eyelid</t>
+  </si>
+  <si>
+    <t>hamartomas of the eyelid</t>
+  </si>
+  <si>
+    <t>verrucous carcinoma of the hypopharynx</t>
+  </si>
+  <si>
+    <t>verrucous carcinoma of the larynx</t>
+  </si>
+  <si>
+    <t>verrucous carcinoma of the trachea</t>
+  </si>
+  <si>
+    <t>verrucous carcinoma of the parapharyngeal space</t>
+  </si>
+  <si>
+    <t>high grade b-cell lymphoma with myc and bcl2 rearrangements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gangliocytoma </t>
+  </si>
+  <si>
+    <t>mixed gangliocytoma-pitnet/adenoma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kshv/hhv8-associated b-cell lymphoid proliferations </t>
+  </si>
+  <si>
+    <t>kshv/hhv8-associated b-cell lymphomas</t>
+  </si>
+  <si>
+    <t>myelodysplastic neoplasm with sf3b1 mutation and thrombocytosis</t>
+  </si>
+  <si>
+    <t>myeloproliferative neoplasm with sf3b1 mutation and thrombocytosis</t>
+  </si>
+  <si>
+    <t>myeloid neoplasms with eosinophilia and defining gene rearrangement</t>
+  </si>
+  <si>
+    <t>lymphoid neoplasms with eosinophilia and defining gene rearrangement</t>
+  </si>
+  <si>
+    <t>nk-lymphoblastic leukaemia/lymphoma</t>
+  </si>
+  <si>
+    <t>nk-lymphoblastic leukaemia</t>
+  </si>
+  <si>
+    <t>nk-lymphoblastic lymphoma</t>
+  </si>
+  <si>
+    <t>nk/t-cell lymphomas</t>
   </si>
 </sst>
 </file>
@@ -8671,12 +9214,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -8691,8 +9240,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -42519,13 +43069,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A40BD13-64D2-A54D-9025-021DFD7EBC52}">
-  <dimension ref="A1:B1611"/>
+  <dimension ref="A1:B1669"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1328" zoomScale="297" zoomScaleNormal="297" workbookViewId="0">
-      <selection activeCell="B1340" sqref="B1340"/>
+    <sheetView tabSelected="1" topLeftCell="A1654" zoomScale="297" zoomScaleNormal="297" workbookViewId="0">
+      <selection activeCell="B1664" sqref="B1664"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="28.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -51270,7 +51823,7 @@
         <v>438</v>
       </c>
       <c r="B1340" t="s">
-        <v>2305</v>
+        <v>2880</v>
       </c>
     </row>
     <row r="1341" spans="1:2" x14ac:dyDescent="0.2">
@@ -51278,2172 +51831,2452 @@
         <v>438</v>
       </c>
       <c r="B1341" t="s">
-        <v>2305</v>
+        <v>2881</v>
       </c>
     </row>
     <row r="1342" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1342">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B1342" t="s">
-        <v>2306</v>
+        <v>2878</v>
       </c>
     </row>
     <row r="1343" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1343">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B1343" t="s">
-        <v>2306</v>
+        <v>2882</v>
       </c>
     </row>
     <row r="1344" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1344">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B1344" t="s">
-        <v>2306</v>
+        <v>2883</v>
       </c>
     </row>
     <row r="1345" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1345">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B1345" t="s">
-        <v>2307</v>
+        <v>2879</v>
       </c>
     </row>
     <row r="1346" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1346">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B1346" t="s">
-        <v>2307</v>
+        <v>2884</v>
       </c>
     </row>
     <row r="1347" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1347">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B1347" t="s">
-        <v>2307</v>
+        <v>2885</v>
       </c>
     </row>
     <row r="1348" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1348">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="B1348" t="s">
-        <v>2308</v>
+        <v>2306</v>
       </c>
     </row>
     <row r="1349" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1349">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="B1349" t="s">
-        <v>2308</v>
+        <v>2886</v>
       </c>
     </row>
     <row r="1350" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1350">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="B1350" t="s">
-        <v>2308</v>
+        <v>2887</v>
       </c>
     </row>
     <row r="1351" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1351">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B1351" t="s">
-        <v>2309</v>
+        <v>2307</v>
       </c>
     </row>
     <row r="1352" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1352">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B1352" t="s">
-        <v>2309</v>
+        <v>2888</v>
       </c>
     </row>
     <row r="1353" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1353">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B1353" t="s">
-        <v>2309</v>
+        <v>2889</v>
       </c>
     </row>
     <row r="1354" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1354">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B1354" t="s">
-        <v>2310</v>
+        <v>2308</v>
       </c>
     </row>
     <row r="1355" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1355">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B1355" t="s">
-        <v>2310</v>
+        <v>2890</v>
       </c>
     </row>
     <row r="1356" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1356">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B1356" t="s">
-        <v>2310</v>
+        <v>2891</v>
       </c>
     </row>
     <row r="1357" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1357">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B1357" t="s">
-        <v>2311</v>
+        <v>2309</v>
       </c>
     </row>
     <row r="1358" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1358">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B1358" t="s">
-        <v>2311</v>
+        <v>1579</v>
       </c>
     </row>
     <row r="1359" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1359">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B1359" t="s">
-        <v>2311</v>
+        <v>2892</v>
       </c>
     </row>
     <row r="1360" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1360">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B1360" t="s">
-        <v>2312</v>
+        <v>2310</v>
       </c>
     </row>
     <row r="1361" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1361">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B1361" t="s">
-        <v>2312</v>
+        <v>2893</v>
       </c>
     </row>
     <row r="1362" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1362">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B1362" t="s">
-        <v>2312</v>
+        <v>2894</v>
       </c>
     </row>
     <row r="1363" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1363">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B1363" t="s">
-        <v>2313</v>
-      </c>
-    </row>
-    <row r="1364" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1364">
-        <v>446</v>
-      </c>
-      <c r="B1364" t="s">
-        <v>2313</v>
-      </c>
-    </row>
-    <row r="1365" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1365">
-        <v>446</v>
-      </c>
-      <c r="B1365" t="s">
-        <v>2313</v>
+        <v>2311</v>
       </c>
     </row>
     <row r="1366" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1366">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B1366" t="s">
-        <v>2314</v>
+        <v>2312</v>
       </c>
     </row>
     <row r="1367" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1367">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B1367" t="s">
-        <v>2314</v>
+        <v>2895</v>
       </c>
     </row>
     <row r="1368" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1368">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B1368" t="s">
-        <v>2314</v>
+        <v>2896</v>
       </c>
     </row>
     <row r="1369" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1369">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B1369" t="s">
-        <v>2315</v>
+        <v>2313</v>
       </c>
     </row>
     <row r="1370" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1370">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B1370" t="s">
-        <v>2315</v>
+        <v>1612</v>
       </c>
     </row>
     <row r="1371" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1371">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B1371" t="s">
-        <v>2315</v>
+        <v>1602</v>
       </c>
     </row>
     <row r="1372" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1372">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B1372" t="s">
-        <v>2316</v>
+        <v>2314</v>
       </c>
     </row>
     <row r="1373" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1373">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B1373" t="s">
-        <v>2316</v>
+        <v>1616</v>
       </c>
     </row>
     <row r="1374" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1374">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B1374" t="s">
-        <v>2316</v>
+        <v>220</v>
       </c>
     </row>
     <row r="1375" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1375">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B1375" t="s">
-        <v>2317</v>
+        <v>2315</v>
       </c>
     </row>
     <row r="1376" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1376">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B1376" t="s">
-        <v>2317</v>
+        <v>2897</v>
       </c>
     </row>
     <row r="1377" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1377">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B1377" t="s">
-        <v>2317</v>
+        <v>2898</v>
       </c>
     </row>
     <row r="1378" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1378">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="B1378" t="s">
-        <v>2318</v>
+        <v>2316</v>
       </c>
     </row>
     <row r="1379" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1379">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="B1379" t="s">
-        <v>2318</v>
+        <v>2899</v>
       </c>
     </row>
     <row r="1380" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1380">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="B1380" t="s">
-        <v>2318</v>
+        <v>2555</v>
       </c>
     </row>
     <row r="1381" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1381">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B1381" t="s">
-        <v>2319</v>
+        <v>2317</v>
       </c>
     </row>
     <row r="1382" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1382">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B1382" t="s">
-        <v>2319</v>
+        <v>2900</v>
       </c>
     </row>
     <row r="1383" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1383">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B1383" t="s">
-        <v>2319</v>
+        <v>2901</v>
       </c>
     </row>
     <row r="1384" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1384">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B1384" t="s">
-        <v>2320</v>
-      </c>
-    </row>
-    <row r="1385" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1385">
-        <v>453</v>
-      </c>
-      <c r="B1385" t="s">
-        <v>2320</v>
-      </c>
-    </row>
-    <row r="1386" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1386">
-        <v>453</v>
-      </c>
-      <c r="B1386" t="s">
-        <v>2320</v>
+        <v>2318</v>
       </c>
     </row>
     <row r="1387" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1387">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="B1387" t="s">
-        <v>2321</v>
+        <v>2319</v>
       </c>
     </row>
     <row r="1388" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1388">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="B1388" t="s">
-        <v>2321</v>
+        <v>2902</v>
       </c>
     </row>
     <row r="1389" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1389">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="B1389" t="s">
-        <v>2321</v>
+        <v>2903</v>
       </c>
     </row>
     <row r="1390" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1390">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="B1390" t="s">
-        <v>2322</v>
+        <v>2320</v>
       </c>
     </row>
     <row r="1391" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1391">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="B1391" t="s">
-        <v>2322</v>
+        <v>2904</v>
       </c>
     </row>
     <row r="1392" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1392">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="B1392" t="s">
-        <v>2322</v>
+        <v>2905</v>
       </c>
     </row>
     <row r="1393" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1393">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B1393" t="s">
-        <v>2323</v>
+        <v>2321</v>
       </c>
     </row>
     <row r="1394" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1394">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B1394" t="s">
-        <v>2323</v>
+        <v>2906</v>
       </c>
     </row>
     <row r="1395" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1395">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B1395" t="s">
-        <v>2323</v>
+        <v>2907</v>
       </c>
     </row>
     <row r="1396" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1396">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="B1396" t="s">
-        <v>2324</v>
+        <v>2322</v>
       </c>
     </row>
     <row r="1397" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1397">
-        <v>457</v>
-      </c>
-      <c r="B1397" t="s">
-        <v>2324</v>
+        <v>455</v>
+      </c>
+      <c r="B1397" s="1" t="s">
+        <v>2908</v>
       </c>
     </row>
     <row r="1398" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1398">
-        <v>457</v>
-      </c>
-      <c r="B1398" t="s">
-        <v>2324</v>
+        <v>455</v>
+      </c>
+      <c r="B1398" s="1" t="s">
+        <v>2909</v>
       </c>
     </row>
     <row r="1399" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1399">
-        <v>458</v>
-      </c>
-      <c r="B1399" t="s">
-        <v>2325</v>
+        <v>455</v>
+      </c>
+      <c r="B1399" s="1" t="s">
+        <v>2910</v>
       </c>
     </row>
     <row r="1400" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1400">
-        <v>458</v>
-      </c>
-      <c r="B1400" t="s">
-        <v>2325</v>
+        <v>455</v>
+      </c>
+      <c r="B1400" s="1" t="s">
+        <v>2911</v>
       </c>
     </row>
     <row r="1401" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1401">
-        <v>458</v>
-      </c>
-      <c r="B1401" t="s">
-        <v>2325</v>
+        <v>455</v>
+      </c>
+      <c r="B1401" s="1" t="s">
+        <v>1714</v>
       </c>
     </row>
     <row r="1402" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1402">
-        <v>459</v>
-      </c>
-      <c r="B1402" t="s">
-        <v>2326</v>
+        <v>455</v>
+      </c>
+      <c r="B1402" s="1" t="s">
+        <v>2912</v>
       </c>
     </row>
     <row r="1403" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1403">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="B1403" t="s">
-        <v>2326</v>
+        <v>2913</v>
       </c>
     </row>
     <row r="1404" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1404">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="B1404" t="s">
-        <v>2326</v>
-      </c>
-    </row>
-    <row r="1405" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1405">
-        <v>460</v>
-      </c>
-      <c r="B1405" t="s">
-        <v>2327</v>
-      </c>
-    </row>
-    <row r="1406" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1406">
-        <v>460</v>
-      </c>
-      <c r="B1406" t="s">
-        <v>2327</v>
+        <v>2914</v>
       </c>
     </row>
     <row r="1407" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1407">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="B1407" t="s">
-        <v>2327</v>
+        <v>2323</v>
       </c>
     </row>
     <row r="1408" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1408">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="B1408" t="s">
-        <v>2328</v>
+        <v>2915</v>
       </c>
     </row>
     <row r="1409" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1409">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="B1409" t="s">
-        <v>2328</v>
+        <v>2916</v>
       </c>
     </row>
     <row r="1410" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1410">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="B1410" t="s">
-        <v>2328</v>
+        <v>2324</v>
       </c>
     </row>
     <row r="1411" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1411">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="B1411" t="s">
-        <v>2329</v>
+        <v>2917</v>
       </c>
     </row>
     <row r="1412" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1412">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="B1412" t="s">
-        <v>2329</v>
+        <v>2918</v>
       </c>
     </row>
     <row r="1413" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1413">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="B1413" t="s">
-        <v>2329</v>
+        <v>2325</v>
       </c>
     </row>
     <row r="1414" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1414">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="B1414" t="s">
-        <v>2330</v>
+        <v>2919</v>
       </c>
     </row>
     <row r="1415" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1415">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="B1415" t="s">
-        <v>2330</v>
+        <v>305</v>
       </c>
     </row>
     <row r="1416" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1416">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="B1416" t="s">
-        <v>2330</v>
+        <v>2326</v>
       </c>
     </row>
     <row r="1417" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1417">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="B1417" t="s">
-        <v>2331</v>
+        <v>2920</v>
       </c>
     </row>
     <row r="1418" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1418">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="B1418" t="s">
-        <v>2331</v>
+        <v>2921</v>
       </c>
     </row>
     <row r="1419" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1419">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="B1419" t="s">
-        <v>2331</v>
+        <v>2922</v>
       </c>
     </row>
     <row r="1420" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1420">
-        <v>465</v>
+        <v>459</v>
       </c>
       <c r="B1420" t="s">
-        <v>2332</v>
+        <v>2923</v>
       </c>
     </row>
     <row r="1421" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1421">
-        <v>465</v>
+        <v>459</v>
       </c>
       <c r="B1421" t="s">
-        <v>2332</v>
+        <v>2924</v>
       </c>
     </row>
     <row r="1422" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1422">
-        <v>465</v>
+        <v>459</v>
       </c>
       <c r="B1422" t="s">
-        <v>2332</v>
+        <v>2925</v>
       </c>
     </row>
     <row r="1423" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1423">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="B1423" t="s">
-        <v>2333</v>
+        <v>2927</v>
       </c>
     </row>
     <row r="1424" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1424">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="B1424" t="s">
-        <v>2333</v>
+        <v>2926</v>
       </c>
     </row>
     <row r="1425" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1425">
-        <v>466</v>
+        <v>460</v>
       </c>
       <c r="B1425" t="s">
-        <v>2333</v>
+        <v>2327</v>
       </c>
     </row>
     <row r="1426" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1426">
-        <v>467</v>
+        <v>460</v>
       </c>
       <c r="B1426" t="s">
-        <v>2334</v>
+        <v>2928</v>
       </c>
     </row>
     <row r="1427" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1427">
-        <v>467</v>
+        <v>460</v>
       </c>
       <c r="B1427" t="s">
-        <v>2334</v>
+        <v>2929</v>
       </c>
     </row>
     <row r="1428" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1428">
-        <v>467</v>
+        <v>461</v>
       </c>
       <c r="B1428" t="s">
-        <v>2334</v>
+        <v>2328</v>
       </c>
     </row>
     <row r="1429" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1429">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="B1429" t="s">
-        <v>2335</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="1430" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1430">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="B1430" t="s">
-        <v>2335</v>
+        <v>2931</v>
       </c>
     </row>
     <row r="1431" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1431">
-        <v>468</v>
+        <v>462</v>
       </c>
       <c r="B1431" t="s">
-        <v>2335</v>
+        <v>2329</v>
       </c>
     </row>
     <row r="1432" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1432">
-        <v>469</v>
+        <v>462</v>
       </c>
       <c r="B1432" t="s">
-        <v>2336</v>
+        <v>2932</v>
       </c>
     </row>
     <row r="1433" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1433">
-        <v>469</v>
+        <v>462</v>
       </c>
       <c r="B1433" t="s">
-        <v>2336</v>
+        <v>2933</v>
       </c>
     </row>
     <row r="1434" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1434">
-        <v>469</v>
+        <v>463</v>
       </c>
       <c r="B1434" t="s">
-        <v>2336</v>
+        <v>2330</v>
       </c>
     </row>
     <row r="1435" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1435">
-        <v>470</v>
+        <v>463</v>
       </c>
       <c r="B1435" t="s">
-        <v>2337</v>
+        <v>2934</v>
       </c>
     </row>
     <row r="1436" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1436">
-        <v>470</v>
+        <v>463</v>
       </c>
       <c r="B1436" t="s">
-        <v>2337</v>
+        <v>2935</v>
       </c>
     </row>
     <row r="1437" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1437">
-        <v>470</v>
+        <v>464</v>
       </c>
       <c r="B1437" t="s">
-        <v>2337</v>
+        <v>2331</v>
       </c>
     </row>
     <row r="1438" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1438">
-        <v>471</v>
+        <v>464</v>
       </c>
       <c r="B1438" t="s">
-        <v>2338</v>
+        <v>2936</v>
       </c>
     </row>
     <row r="1439" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1439">
-        <v>471</v>
+        <v>464</v>
       </c>
       <c r="B1439" t="s">
-        <v>2338</v>
+        <v>2937</v>
       </c>
     </row>
     <row r="1440" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1440">
-        <v>471</v>
+        <v>465</v>
       </c>
       <c r="B1440" t="s">
-        <v>2338</v>
+        <v>2332</v>
       </c>
     </row>
     <row r="1441" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1441">
-        <v>472</v>
+        <v>465</v>
       </c>
       <c r="B1441" t="s">
-        <v>2339</v>
+        <v>2938</v>
       </c>
     </row>
     <row r="1442" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1442">
-        <v>472</v>
+        <v>465</v>
       </c>
       <c r="B1442" t="s">
-        <v>2339</v>
+        <v>2939</v>
       </c>
     </row>
     <row r="1443" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1443">
-        <v>472</v>
+        <v>466</v>
       </c>
       <c r="B1443" t="s">
-        <v>2339</v>
+        <v>2333</v>
       </c>
     </row>
     <row r="1444" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1444">
-        <v>473</v>
+        <v>466</v>
       </c>
       <c r="B1444" t="s">
-        <v>2340</v>
+        <v>2940</v>
       </c>
     </row>
     <row r="1445" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1445">
-        <v>473</v>
+        <v>466</v>
       </c>
       <c r="B1445" t="s">
-        <v>2340</v>
+        <v>2941</v>
       </c>
     </row>
     <row r="1446" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1446">
-        <v>473</v>
+        <v>467</v>
       </c>
       <c r="B1446" t="s">
-        <v>2340</v>
+        <v>2334</v>
       </c>
     </row>
     <row r="1447" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1447">
-        <v>474</v>
+        <v>467</v>
       </c>
       <c r="B1447" t="s">
-        <v>2341</v>
+        <v>2942</v>
       </c>
     </row>
     <row r="1448" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1448">
-        <v>474</v>
+        <v>467</v>
       </c>
       <c r="B1448" t="s">
-        <v>2341</v>
+        <v>2943</v>
       </c>
     </row>
     <row r="1449" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1449">
-        <v>474</v>
+        <v>468</v>
       </c>
       <c r="B1449" t="s">
-        <v>2341</v>
-      </c>
-    </row>
-    <row r="1450" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1450">
-        <v>475</v>
-      </c>
-      <c r="B1450" t="s">
-        <v>2342</v>
-      </c>
-    </row>
-    <row r="1451" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1451">
-        <v>475</v>
-      </c>
-      <c r="B1451" t="s">
-        <v>2342</v>
+        <v>2335</v>
       </c>
     </row>
     <row r="1452" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1452">
-        <v>475</v>
+        <v>469</v>
       </c>
       <c r="B1452" t="s">
-        <v>2342</v>
+        <v>2336</v>
       </c>
     </row>
     <row r="1453" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1453">
-        <v>476</v>
+        <v>469</v>
       </c>
       <c r="B1453" t="s">
-        <v>2343</v>
+        <v>2944</v>
       </c>
     </row>
     <row r="1454" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1454">
-        <v>476</v>
+        <v>469</v>
       </c>
       <c r="B1454" t="s">
-        <v>2343</v>
+        <v>2945</v>
       </c>
     </row>
     <row r="1455" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1455">
-        <v>476</v>
+        <v>470</v>
       </c>
       <c r="B1455" t="s">
-        <v>2343</v>
+        <v>2337</v>
       </c>
     </row>
     <row r="1456" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1456">
-        <v>477</v>
+        <v>470</v>
       </c>
       <c r="B1456" t="s">
-        <v>2344</v>
+        <v>2946</v>
       </c>
     </row>
     <row r="1457" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1457">
-        <v>477</v>
+        <v>470</v>
       </c>
       <c r="B1457" t="s">
-        <v>2344</v>
+        <v>2947</v>
       </c>
     </row>
     <row r="1458" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1458">
-        <v>477</v>
+        <v>471</v>
       </c>
       <c r="B1458" t="s">
-        <v>2344</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="1459" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1459">
-        <v>478</v>
+        <v>471</v>
       </c>
       <c r="B1459" t="s">
-        <v>2345</v>
+        <v>2948</v>
       </c>
     </row>
     <row r="1460" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1460">
-        <v>478</v>
+        <v>471</v>
       </c>
       <c r="B1460" t="s">
-        <v>2345</v>
+        <v>2949</v>
       </c>
     </row>
     <row r="1461" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1461">
-        <v>478</v>
+        <v>472</v>
       </c>
       <c r="B1461" t="s">
-        <v>2345</v>
+        <v>2339</v>
       </c>
     </row>
     <row r="1462" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1462">
-        <v>479</v>
+        <v>472</v>
       </c>
       <c r="B1462" t="s">
-        <v>2346</v>
+        <v>2950</v>
       </c>
     </row>
     <row r="1463" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1463">
-        <v>479</v>
+        <v>472</v>
       </c>
       <c r="B1463" t="s">
-        <v>2346</v>
+        <v>2951</v>
       </c>
     </row>
     <row r="1464" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1464">
-        <v>479</v>
+        <v>473</v>
       </c>
       <c r="B1464" t="s">
-        <v>2346</v>
+        <v>2340</v>
       </c>
     </row>
     <row r="1465" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1465">
-        <v>480</v>
+        <v>473</v>
       </c>
       <c r="B1465" t="s">
-        <v>2347</v>
+        <v>2952</v>
       </c>
     </row>
     <row r="1466" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1466">
-        <v>480</v>
+        <v>473</v>
       </c>
       <c r="B1466" t="s">
-        <v>2347</v>
+        <v>2953</v>
       </c>
     </row>
     <row r="1467" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1467">
-        <v>480</v>
+        <v>474</v>
       </c>
       <c r="B1467" t="s">
-        <v>2347</v>
+        <v>2341</v>
       </c>
     </row>
     <row r="1468" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1468">
-        <v>481</v>
+        <v>474</v>
       </c>
       <c r="B1468" t="s">
-        <v>2348</v>
+        <v>2954</v>
       </c>
     </row>
     <row r="1469" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1469">
-        <v>481</v>
+        <v>474</v>
       </c>
       <c r="B1469" t="s">
-        <v>2348</v>
+        <v>2955</v>
       </c>
     </row>
     <row r="1470" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1470">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="B1470" t="s">
-        <v>2348</v>
+        <v>2342</v>
       </c>
     </row>
     <row r="1471" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1471">
-        <v>482</v>
+        <v>475</v>
       </c>
       <c r="B1471" t="s">
-        <v>2349</v>
+        <v>2956</v>
       </c>
     </row>
     <row r="1472" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1472">
-        <v>482</v>
+        <v>475</v>
       </c>
       <c r="B1472" t="s">
-        <v>2349</v>
+        <v>2957</v>
       </c>
     </row>
     <row r="1473" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1473">
-        <v>482</v>
+        <v>476</v>
       </c>
       <c r="B1473" t="s">
-        <v>2349</v>
+        <v>2343</v>
       </c>
     </row>
     <row r="1474" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1474">
-        <v>483</v>
+        <v>476</v>
       </c>
       <c r="B1474" t="s">
-        <v>2350</v>
+        <v>2958</v>
       </c>
     </row>
     <row r="1475" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1475">
-        <v>483</v>
+        <v>476</v>
       </c>
       <c r="B1475" t="s">
-        <v>2350</v>
+        <v>2959</v>
       </c>
     </row>
     <row r="1476" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1476">
-        <v>483</v>
+        <v>477</v>
       </c>
       <c r="B1476" t="s">
-        <v>2350</v>
+        <v>2344</v>
       </c>
     </row>
     <row r="1477" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1477">
-        <v>484</v>
+        <v>477</v>
       </c>
       <c r="B1477" t="s">
-        <v>2351</v>
+        <v>2960</v>
       </c>
     </row>
     <row r="1478" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1478">
-        <v>484</v>
+        <v>477</v>
       </c>
       <c r="B1478" t="s">
-        <v>2351</v>
+        <v>2961</v>
       </c>
     </row>
     <row r="1479" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1479">
-        <v>484</v>
+        <v>478</v>
       </c>
       <c r="B1479" t="s">
-        <v>2351</v>
+        <v>2345</v>
       </c>
     </row>
     <row r="1480" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1480">
-        <v>485</v>
+        <v>478</v>
       </c>
       <c r="B1480" t="s">
-        <v>2352</v>
+        <v>2962</v>
       </c>
     </row>
     <row r="1481" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1481">
-        <v>485</v>
+        <v>478</v>
       </c>
       <c r="B1481" t="s">
-        <v>2352</v>
+        <v>2963</v>
       </c>
     </row>
     <row r="1482" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1482">
-        <v>485</v>
+        <v>479</v>
       </c>
       <c r="B1482" t="s">
-        <v>2352</v>
+        <v>2346</v>
       </c>
     </row>
     <row r="1483" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1483">
-        <v>486</v>
+        <v>479</v>
       </c>
       <c r="B1483" t="s">
-        <v>2353</v>
+        <v>2964</v>
       </c>
     </row>
     <row r="1484" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1484">
-        <v>486</v>
+        <v>479</v>
       </c>
       <c r="B1484" t="s">
-        <v>2353</v>
+        <v>2965</v>
       </c>
     </row>
     <row r="1485" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1485">
-        <v>486</v>
+        <v>480</v>
       </c>
       <c r="B1485" t="s">
-        <v>2353</v>
+        <v>2347</v>
       </c>
     </row>
     <row r="1486" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1486">
-        <v>487</v>
+        <v>480</v>
       </c>
       <c r="B1486" t="s">
-        <v>2354</v>
+        <v>2966</v>
       </c>
     </row>
     <row r="1487" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1487">
-        <v>487</v>
+        <v>480</v>
       </c>
       <c r="B1487" t="s">
-        <v>2354</v>
+        <v>2967</v>
       </c>
     </row>
     <row r="1488" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1488">
-        <v>487</v>
+        <v>481</v>
       </c>
       <c r="B1488" t="s">
-        <v>2354</v>
+        <v>2348</v>
       </c>
     </row>
     <row r="1489" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1489">
-        <v>488</v>
+        <v>481</v>
       </c>
       <c r="B1489" t="s">
-        <v>2355</v>
+        <v>2968</v>
       </c>
     </row>
     <row r="1490" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1490">
-        <v>488</v>
+        <v>481</v>
       </c>
       <c r="B1490" t="s">
-        <v>2355</v>
+        <v>2969</v>
       </c>
     </row>
     <row r="1491" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1491">
-        <v>488</v>
+        <v>482</v>
       </c>
       <c r="B1491" t="s">
-        <v>2355</v>
-      </c>
-    </row>
-    <row r="1492" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1492">
-        <v>489</v>
-      </c>
-      <c r="B1492" t="s">
-        <v>2356</v>
-      </c>
-    </row>
-    <row r="1493" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1493">
-        <v>489</v>
-      </c>
-      <c r="B1493" t="s">
-        <v>2356</v>
+        <v>2349</v>
       </c>
     </row>
     <row r="1494" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1494">
-        <v>489</v>
+        <v>483</v>
       </c>
       <c r="B1494" t="s">
-        <v>2356</v>
+        <v>2350</v>
       </c>
     </row>
     <row r="1495" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1495">
-        <v>490</v>
+        <v>483</v>
       </c>
       <c r="B1495" t="s">
-        <v>2357</v>
+        <v>2970</v>
       </c>
     </row>
     <row r="1496" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1496">
-        <v>490</v>
+        <v>483</v>
       </c>
       <c r="B1496" t="s">
-        <v>2357</v>
+        <v>2875</v>
       </c>
     </row>
     <row r="1497" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1497">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="B1497" t="s">
-        <v>2357</v>
+        <v>2351</v>
       </c>
     </row>
     <row r="1498" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1498">
-        <v>491</v>
+        <v>484</v>
       </c>
       <c r="B1498" t="s">
-        <v>2358</v>
+        <v>1842</v>
       </c>
     </row>
     <row r="1499" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1499">
-        <v>491</v>
+        <v>484</v>
       </c>
       <c r="B1499" t="s">
-        <v>2358</v>
+        <v>1371</v>
       </c>
     </row>
     <row r="1500" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1500">
-        <v>491</v>
+        <v>485</v>
       </c>
       <c r="B1500" t="s">
-        <v>2358</v>
+        <v>2352</v>
       </c>
     </row>
     <row r="1501" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1501">
-        <v>492</v>
+        <v>485</v>
       </c>
       <c r="B1501" t="s">
-        <v>2359</v>
+        <v>2971</v>
       </c>
     </row>
     <row r="1502" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1502">
-        <v>492</v>
+        <v>485</v>
       </c>
       <c r="B1502" t="s">
-        <v>2359</v>
+        <v>2972</v>
       </c>
     </row>
     <row r="1503" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1503">
-        <v>492</v>
+        <v>486</v>
       </c>
       <c r="B1503" t="s">
-        <v>2359</v>
+        <v>2353</v>
       </c>
     </row>
     <row r="1504" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1504">
-        <v>493</v>
+        <v>486</v>
       </c>
       <c r="B1504" t="s">
-        <v>2360</v>
+        <v>2973</v>
       </c>
     </row>
     <row r="1505" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1505">
-        <v>493</v>
+        <v>486</v>
       </c>
       <c r="B1505" t="s">
-        <v>2360</v>
+        <v>2974</v>
       </c>
     </row>
     <row r="1506" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1506">
-        <v>493</v>
+        <v>487</v>
       </c>
       <c r="B1506" t="s">
-        <v>2360</v>
+        <v>2354</v>
       </c>
     </row>
     <row r="1507" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1507">
-        <v>494</v>
+        <v>487</v>
       </c>
       <c r="B1507" t="s">
-        <v>2361</v>
+        <v>2975</v>
       </c>
     </row>
     <row r="1508" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1508">
-        <v>494</v>
+        <v>487</v>
       </c>
       <c r="B1508" t="s">
-        <v>2361</v>
+        <v>2976</v>
       </c>
     </row>
     <row r="1509" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1509">
-        <v>494</v>
+        <v>488</v>
       </c>
       <c r="B1509" t="s">
-        <v>2361</v>
+        <v>2355</v>
       </c>
     </row>
     <row r="1510" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1510">
-        <v>495</v>
+        <v>488</v>
       </c>
       <c r="B1510" t="s">
-        <v>2362</v>
+        <v>2979</v>
       </c>
     </row>
     <row r="1511" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1511">
-        <v>495</v>
+        <v>488</v>
       </c>
       <c r="B1511" t="s">
-        <v>2362</v>
+        <v>2977</v>
       </c>
     </row>
     <row r="1512" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1512">
-        <v>495</v>
+        <v>488</v>
       </c>
       <c r="B1512" t="s">
-        <v>2362</v>
+        <v>2978</v>
       </c>
     </row>
     <row r="1513" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1513">
-        <v>496</v>
+        <v>489</v>
       </c>
       <c r="B1513" t="s">
-        <v>2363</v>
+        <v>2356</v>
       </c>
     </row>
     <row r="1514" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1514">
-        <v>496</v>
+        <v>489</v>
       </c>
       <c r="B1514" t="s">
-        <v>2363</v>
+        <v>2984</v>
       </c>
     </row>
     <row r="1515" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1515">
-        <v>496</v>
+        <v>489</v>
       </c>
       <c r="B1515" t="s">
-        <v>2363</v>
+        <v>2980</v>
       </c>
     </row>
     <row r="1516" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1516">
-        <v>497</v>
+        <v>489</v>
       </c>
       <c r="B1516" t="s">
-        <v>2364</v>
+        <v>2983</v>
       </c>
     </row>
     <row r="1517" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1517">
-        <v>497</v>
+        <v>490</v>
       </c>
       <c r="B1517" t="s">
-        <v>2364</v>
+        <v>2357</v>
       </c>
     </row>
     <row r="1518" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1518">
-        <v>497</v>
+        <v>490</v>
       </c>
       <c r="B1518" t="s">
-        <v>2364</v>
+        <v>2985</v>
       </c>
     </row>
     <row r="1519" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1519">
-        <v>498</v>
+        <v>490</v>
       </c>
       <c r="B1519" t="s">
-        <v>2365</v>
+        <v>2986</v>
       </c>
     </row>
     <row r="1520" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1520">
-        <v>498</v>
+        <v>491</v>
       </c>
       <c r="B1520" t="s">
-        <v>2365</v>
+        <v>2358</v>
       </c>
     </row>
     <row r="1521" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1521">
-        <v>498</v>
+        <v>491</v>
       </c>
       <c r="B1521" t="s">
-        <v>2365</v>
+        <v>2989</v>
       </c>
     </row>
     <row r="1522" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1522">
-        <v>499</v>
+        <v>491</v>
       </c>
       <c r="B1522" t="s">
-        <v>2366</v>
+        <v>2987</v>
       </c>
     </row>
     <row r="1523" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1523">
-        <v>499</v>
+        <v>491</v>
       </c>
       <c r="B1523" t="s">
-        <v>2366</v>
+        <v>2988</v>
       </c>
     </row>
     <row r="1524" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1524">
-        <v>499</v>
+        <v>492</v>
       </c>
       <c r="B1524" t="s">
-        <v>2366</v>
-      </c>
-    </row>
-    <row r="1525" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1525">
-        <v>500</v>
-      </c>
-      <c r="B1525" t="s">
-        <v>2367</v>
-      </c>
-    </row>
-    <row r="1526" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1526">
-        <v>500</v>
-      </c>
-      <c r="B1526" t="s">
-        <v>2367</v>
+        <v>2359</v>
       </c>
     </row>
     <row r="1527" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1527">
-        <v>500</v>
+        <v>493</v>
       </c>
       <c r="B1527" t="s">
-        <v>2367</v>
+        <v>2360</v>
       </c>
     </row>
     <row r="1528" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1528">
-        <v>501</v>
+        <v>493</v>
       </c>
       <c r="B1528" t="s">
-        <v>2368</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="1529" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1529">
-        <v>501</v>
+        <v>493</v>
       </c>
       <c r="B1529" t="s">
-        <v>2368</v>
+        <v>2702</v>
       </c>
     </row>
     <row r="1530" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1530">
-        <v>501</v>
+        <v>493</v>
       </c>
       <c r="B1530" t="s">
-        <v>2368</v>
+        <v>2990</v>
       </c>
     </row>
     <row r="1531" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1531">
-        <v>502</v>
+        <v>494</v>
       </c>
       <c r="B1531" t="s">
-        <v>2369</v>
-      </c>
-    </row>
-    <row r="1532" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1532">
-        <v>502</v>
-      </c>
-      <c r="B1532" t="s">
-        <v>2369</v>
-      </c>
-    </row>
-    <row r="1533" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1533">
-        <v>502</v>
-      </c>
-      <c r="B1533" t="s">
-        <v>2369</v>
+        <v>2361</v>
       </c>
     </row>
     <row r="1534" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1534">
-        <v>503</v>
+        <v>495</v>
       </c>
       <c r="B1534" t="s">
-        <v>2370</v>
+        <v>2362</v>
       </c>
     </row>
     <row r="1535" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1535">
-        <v>503</v>
+        <v>495</v>
       </c>
       <c r="B1535" t="s">
-        <v>2370</v>
+        <v>2716</v>
       </c>
     </row>
     <row r="1536" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1536">
-        <v>503</v>
+        <v>495</v>
       </c>
       <c r="B1536" t="s">
-        <v>2370</v>
+        <v>2991</v>
       </c>
     </row>
     <row r="1537" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1537">
-        <v>504</v>
+        <v>495</v>
       </c>
       <c r="B1537" t="s">
-        <v>2371</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="1538" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1538">
-        <v>504</v>
+        <v>496</v>
       </c>
       <c r="B1538" t="s">
-        <v>2371</v>
+        <v>2363</v>
       </c>
     </row>
     <row r="1539" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1539">
-        <v>504</v>
+        <v>496</v>
       </c>
       <c r="B1539" t="s">
-        <v>2371</v>
+        <v>2995</v>
       </c>
     </row>
     <row r="1540" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1540">
-        <v>505</v>
+        <v>496</v>
       </c>
       <c r="B1540" t="s">
-        <v>2372</v>
+        <v>2992</v>
       </c>
     </row>
     <row r="1541" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1541">
-        <v>505</v>
+        <v>496</v>
       </c>
       <c r="B1541" t="s">
-        <v>2372</v>
+        <v>2993</v>
       </c>
     </row>
     <row r="1542" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1542">
-        <v>505</v>
+        <v>496</v>
       </c>
       <c r="B1542" t="s">
-        <v>2372</v>
+        <v>2994</v>
       </c>
     </row>
     <row r="1543" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1543">
-        <v>506</v>
+        <v>497</v>
       </c>
       <c r="B1543" t="s">
-        <v>2373</v>
+        <v>2364</v>
       </c>
     </row>
     <row r="1544" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1544">
-        <v>506</v>
+        <v>497</v>
       </c>
       <c r="B1544" t="s">
-        <v>2373</v>
+        <v>2996</v>
       </c>
     </row>
     <row r="1545" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1545">
-        <v>506</v>
+        <v>497</v>
       </c>
       <c r="B1545" t="s">
-        <v>2373</v>
+        <v>2997</v>
       </c>
     </row>
     <row r="1546" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1546">
-        <v>507</v>
+        <v>497</v>
       </c>
       <c r="B1546" t="s">
-        <v>2374</v>
+        <v>2998</v>
       </c>
     </row>
     <row r="1547" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1547">
-        <v>507</v>
+        <v>498</v>
       </c>
       <c r="B1547" t="s">
-        <v>2374</v>
+        <v>2365</v>
       </c>
     </row>
     <row r="1548" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1548">
-        <v>507</v>
+        <v>498</v>
       </c>
       <c r="B1548" t="s">
-        <v>2374</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="1549" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1549">
-        <v>508</v>
+        <v>498</v>
       </c>
       <c r="B1549" t="s">
-        <v>2375</v>
+        <v>2988</v>
       </c>
     </row>
     <row r="1550" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1550">
-        <v>508</v>
+        <v>498</v>
       </c>
       <c r="B1550" t="s">
-        <v>2375</v>
+        <v>2999</v>
       </c>
     </row>
     <row r="1551" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1551">
-        <v>508</v>
+        <v>499</v>
       </c>
       <c r="B1551" t="s">
-        <v>2375</v>
+        <v>2366</v>
       </c>
     </row>
     <row r="1552" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1552">
-        <v>509</v>
+        <v>499</v>
       </c>
       <c r="B1552" t="s">
-        <v>2376</v>
+        <v>2988</v>
       </c>
     </row>
     <row r="1553" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1553">
-        <v>509</v>
+        <v>499</v>
       </c>
       <c r="B1553" t="s">
-        <v>2376</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="1554" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1554">
-        <v>509</v>
+        <v>499</v>
       </c>
       <c r="B1554" t="s">
-        <v>2376</v>
+        <v>3001</v>
       </c>
     </row>
     <row r="1555" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1555">
-        <v>510</v>
+        <v>500</v>
       </c>
       <c r="B1555" t="s">
-        <v>2377</v>
+        <v>2367</v>
       </c>
     </row>
     <row r="1556" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1556">
-        <v>510</v>
+        <v>500</v>
       </c>
       <c r="B1556" t="s">
-        <v>2377</v>
+        <v>3002</v>
       </c>
     </row>
     <row r="1557" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1557">
-        <v>510</v>
+        <v>500</v>
       </c>
       <c r="B1557" t="s">
-        <v>2377</v>
+        <v>2981</v>
       </c>
     </row>
     <row r="1558" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1558">
-        <v>511</v>
+        <v>500</v>
       </c>
       <c r="B1558" t="s">
-        <v>2378</v>
+        <v>2982</v>
       </c>
     </row>
     <row r="1559" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1559">
-        <v>511</v>
+        <v>501</v>
       </c>
       <c r="B1559" t="s">
-        <v>2378</v>
-      </c>
-    </row>
-    <row r="1560" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1560">
-        <v>511</v>
-      </c>
-      <c r="B1560" t="s">
-        <v>2378</v>
-      </c>
-    </row>
-    <row r="1561" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1561">
-        <v>512</v>
-      </c>
-      <c r="B1561" t="s">
-        <v>2379</v>
+        <v>2368</v>
       </c>
     </row>
     <row r="1562" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1562">
-        <v>512</v>
+        <v>502</v>
       </c>
       <c r="B1562" t="s">
-        <v>2379</v>
-      </c>
-    </row>
-    <row r="1563" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1563">
-        <v>512</v>
-      </c>
-      <c r="B1563" t="s">
-        <v>2379</v>
-      </c>
-    </row>
-    <row r="1564" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1564">
-        <v>513</v>
-      </c>
-      <c r="B1564" t="s">
-        <v>2380</v>
+        <v>2369</v>
       </c>
     </row>
     <row r="1565" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1565">
-        <v>513</v>
+        <v>503</v>
       </c>
       <c r="B1565" t="s">
-        <v>2380</v>
+        <v>2370</v>
       </c>
     </row>
     <row r="1566" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1566">
-        <v>513</v>
+        <v>503</v>
       </c>
       <c r="B1566" t="s">
-        <v>2380</v>
+        <v>3003</v>
       </c>
     </row>
     <row r="1567" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1567">
-        <v>514</v>
+        <v>503</v>
       </c>
       <c r="B1567" t="s">
-        <v>2381</v>
+        <v>3004</v>
       </c>
     </row>
     <row r="1568" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1568">
-        <v>514</v>
+        <v>503</v>
       </c>
       <c r="B1568" t="s">
-        <v>2381</v>
+        <v>3005</v>
       </c>
     </row>
     <row r="1569" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1569">
-        <v>514</v>
+        <v>504</v>
       </c>
       <c r="B1569" t="s">
-        <v>2381</v>
+        <v>2371</v>
       </c>
     </row>
     <row r="1570" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1570">
-        <v>515</v>
+        <v>504</v>
       </c>
       <c r="B1570" t="s">
-        <v>2382</v>
+        <v>3009</v>
       </c>
     </row>
     <row r="1571" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1571">
-        <v>515</v>
+        <v>504</v>
       </c>
       <c r="B1571" t="s">
-        <v>2382</v>
+        <v>3006</v>
       </c>
     </row>
     <row r="1572" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1572">
-        <v>515</v>
+        <v>504</v>
       </c>
       <c r="B1572" t="s">
-        <v>2382</v>
+        <v>3007</v>
       </c>
     </row>
     <row r="1573" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1573">
-        <v>516</v>
+        <v>504</v>
       </c>
       <c r="B1573" t="s">
-        <v>2383</v>
+        <v>3008</v>
       </c>
     </row>
     <row r="1574" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1574">
-        <v>516</v>
+        <v>505</v>
       </c>
       <c r="B1574" t="s">
-        <v>2383</v>
+        <v>2372</v>
       </c>
     </row>
     <row r="1575" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1575">
-        <v>516</v>
+        <v>505</v>
       </c>
       <c r="B1575" t="s">
-        <v>2383</v>
+        <v>3010</v>
       </c>
     </row>
     <row r="1576" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1576">
-        <v>517</v>
+        <v>505</v>
       </c>
       <c r="B1576" t="s">
-        <v>2384</v>
+        <v>1955</v>
       </c>
     </row>
     <row r="1577" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1577">
-        <v>517</v>
+        <v>506</v>
       </c>
       <c r="B1577" t="s">
-        <v>2384</v>
+        <v>2373</v>
       </c>
     </row>
     <row r="1578" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1578">
-        <v>517</v>
+        <v>506</v>
       </c>
       <c r="B1578" t="s">
-        <v>2384</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="1579" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1579">
-        <v>518</v>
+        <v>506</v>
       </c>
       <c r="B1579" t="s">
-        <v>2385</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="1580" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1580">
-        <v>518</v>
+        <v>506</v>
       </c>
       <c r="B1580" t="s">
-        <v>2385</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="1581" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1581">
-        <v>518</v>
+        <v>507</v>
       </c>
       <c r="B1581" t="s">
-        <v>2385</v>
+        <v>2374</v>
       </c>
     </row>
     <row r="1582" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1582">
-        <v>519</v>
+        <v>507</v>
       </c>
       <c r="B1582" t="s">
-        <v>2386</v>
+        <v>3011</v>
       </c>
     </row>
     <row r="1583" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1583">
-        <v>519</v>
+        <v>507</v>
       </c>
       <c r="B1583" t="s">
-        <v>2386</v>
+        <v>3012</v>
       </c>
     </row>
     <row r="1584" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1584">
-        <v>519</v>
+        <v>507</v>
       </c>
       <c r="B1584" t="s">
-        <v>2386</v>
+        <v>3013</v>
       </c>
     </row>
     <row r="1585" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1585">
-        <v>520</v>
+        <v>508</v>
       </c>
       <c r="B1585" t="s">
-        <v>2387</v>
+        <v>2375</v>
       </c>
     </row>
     <row r="1586" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1586">
-        <v>520</v>
+        <v>508</v>
       </c>
       <c r="B1586" t="s">
-        <v>2387</v>
+        <v>2870</v>
       </c>
     </row>
     <row r="1587" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1587">
-        <v>520</v>
+        <v>508</v>
       </c>
       <c r="B1587" t="s">
-        <v>2387</v>
+        <v>3016</v>
       </c>
     </row>
     <row r="1588" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1588">
-        <v>521</v>
+        <v>508</v>
       </c>
       <c r="B1588" t="s">
-        <v>2388</v>
+        <v>3017</v>
       </c>
     </row>
     <row r="1589" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1589">
-        <v>521</v>
+        <v>508</v>
       </c>
       <c r="B1589" t="s">
-        <v>2388</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="1590" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1590">
-        <v>521</v>
+        <v>508</v>
       </c>
       <c r="B1590" t="s">
-        <v>2388</v>
+        <v>3014</v>
       </c>
     </row>
     <row r="1591" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1591">
-        <v>522</v>
+        <v>508</v>
       </c>
       <c r="B1591" t="s">
-        <v>2389</v>
+        <v>3015</v>
       </c>
     </row>
     <row r="1592" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1592">
-        <v>522</v>
+        <v>509</v>
       </c>
       <c r="B1592" t="s">
-        <v>2389</v>
+        <v>2376</v>
       </c>
     </row>
     <row r="1593" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1593">
-        <v>522</v>
+        <v>509</v>
       </c>
       <c r="B1593" t="s">
-        <v>2389</v>
+        <v>2817</v>
       </c>
     </row>
     <row r="1594" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1594">
-        <v>523</v>
+        <v>509</v>
       </c>
       <c r="B1594" t="s">
-        <v>2390</v>
+        <v>3018</v>
       </c>
     </row>
     <row r="1595" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1595">
-        <v>523</v>
+        <v>509</v>
       </c>
       <c r="B1595" t="s">
-        <v>2390</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="1596" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1596">
-        <v>523</v>
+        <v>510</v>
       </c>
       <c r="B1596" t="s">
-        <v>2390</v>
+        <v>2377</v>
       </c>
     </row>
     <row r="1597" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1597">
-        <v>524</v>
+        <v>510</v>
       </c>
       <c r="B1597" t="s">
-        <v>2391</v>
+        <v>3019</v>
       </c>
     </row>
     <row r="1598" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1598">
-        <v>524</v>
+        <v>510</v>
       </c>
       <c r="B1598" t="s">
-        <v>2391</v>
+        <v>3020</v>
       </c>
     </row>
     <row r="1599" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1599">
-        <v>524</v>
+        <v>510</v>
       </c>
       <c r="B1599" t="s">
-        <v>2391</v>
+        <v>3021</v>
       </c>
     </row>
     <row r="1600" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1600">
-        <v>525</v>
+        <v>511</v>
       </c>
       <c r="B1600" t="s">
-        <v>2392</v>
+        <v>2378</v>
       </c>
     </row>
     <row r="1601" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1601">
-        <v>525</v>
+        <v>511</v>
       </c>
       <c r="B1601" t="s">
-        <v>2392</v>
+        <v>3022</v>
       </c>
     </row>
     <row r="1602" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1602">
-        <v>525</v>
+        <v>511</v>
       </c>
       <c r="B1602" t="s">
-        <v>2392</v>
+        <v>3023</v>
       </c>
     </row>
     <row r="1603" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1603">
-        <v>526</v>
+        <v>511</v>
       </c>
       <c r="B1603" t="s">
-        <v>2393</v>
+        <v>3024</v>
       </c>
     </row>
     <row r="1604" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1604">
-        <v>526</v>
+        <v>512</v>
       </c>
       <c r="B1604" t="s">
-        <v>2393</v>
+        <v>2379</v>
       </c>
     </row>
     <row r="1605" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1605">
-        <v>526</v>
+        <v>512</v>
       </c>
       <c r="B1605" t="s">
-        <v>2393</v>
+        <v>3025</v>
       </c>
     </row>
     <row r="1606" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1606">
-        <v>527</v>
+        <v>512</v>
       </c>
       <c r="B1606" t="s">
-        <v>2394</v>
+        <v>3026</v>
       </c>
     </row>
     <row r="1607" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1607">
-        <v>527</v>
+        <v>512</v>
       </c>
       <c r="B1607" t="s">
-        <v>2394</v>
+        <v>3027</v>
       </c>
     </row>
     <row r="1608" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1608">
-        <v>527</v>
+        <v>513</v>
       </c>
       <c r="B1608" t="s">
-        <v>2394</v>
+        <v>2380</v>
       </c>
     </row>
     <row r="1609" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1609">
-        <v>528</v>
+        <v>513</v>
       </c>
       <c r="B1609" t="s">
-        <v>2395</v>
+        <v>3028</v>
       </c>
     </row>
     <row r="1610" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1610">
-        <v>528</v>
+        <v>513</v>
       </c>
       <c r="B1610" t="s">
-        <v>2395</v>
+        <v>1548</v>
       </c>
     </row>
     <row r="1611" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1611">
+        <v>513</v>
+      </c>
+      <c r="B1611" t="s">
+        <v>1546</v>
+      </c>
+    </row>
+    <row r="1612" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1612">
+        <v>514</v>
+      </c>
+      <c r="B1612" t="s">
+        <v>2381</v>
+      </c>
+    </row>
+    <row r="1613" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1613">
+        <v>514</v>
+      </c>
+      <c r="B1613" t="s">
+        <v>3029</v>
+      </c>
+    </row>
+    <row r="1614" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1614">
+        <v>514</v>
+      </c>
+      <c r="B1614" t="s">
+        <v>3030</v>
+      </c>
+    </row>
+    <row r="1615" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1615">
+        <v>515</v>
+      </c>
+      <c r="B1615" t="s">
+        <v>2382</v>
+      </c>
+    </row>
+    <row r="1616" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1616">
+        <v>515</v>
+      </c>
+      <c r="B1616" t="s">
+        <v>3031</v>
+      </c>
+    </row>
+    <row r="1617" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1617">
+        <v>515</v>
+      </c>
+      <c r="B1617" t="s">
+        <v>3032</v>
+      </c>
+    </row>
+    <row r="1618" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1618">
+        <v>515</v>
+      </c>
+      <c r="B1618" t="s">
+        <v>3033</v>
+      </c>
+    </row>
+    <row r="1619" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1619">
+        <v>516</v>
+      </c>
+      <c r="B1619" t="s">
+        <v>2383</v>
+      </c>
+    </row>
+    <row r="1620" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1620">
+        <v>516</v>
+      </c>
+      <c r="B1620" t="s">
+        <v>3037</v>
+      </c>
+    </row>
+    <row r="1621" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1621">
+        <v>516</v>
+      </c>
+      <c r="B1621" t="s">
+        <v>3034</v>
+      </c>
+    </row>
+    <row r="1622" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1622">
+        <v>516</v>
+      </c>
+      <c r="B1622" t="s">
+        <v>3035</v>
+      </c>
+    </row>
+    <row r="1623" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1623">
+        <v>516</v>
+      </c>
+      <c r="B1623" t="s">
+        <v>3036</v>
+      </c>
+    </row>
+    <row r="1624" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1624">
+        <v>517</v>
+      </c>
+      <c r="B1624" t="s">
+        <v>2384</v>
+      </c>
+    </row>
+    <row r="1625" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1625">
+        <v>517</v>
+      </c>
+      <c r="B1625" t="s">
+        <v>3038</v>
+      </c>
+    </row>
+    <row r="1626" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1626">
+        <v>517</v>
+      </c>
+      <c r="B1626" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="1627" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1627">
+        <v>517</v>
+      </c>
+      <c r="B1627" t="s">
+        <v>3039</v>
+      </c>
+    </row>
+    <row r="1628" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1628">
+        <v>518</v>
+      </c>
+      <c r="B1628" t="s">
+        <v>2385</v>
+      </c>
+    </row>
+    <row r="1629" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1629">
+        <v>518</v>
+      </c>
+      <c r="B1629" t="s">
+        <v>3040</v>
+      </c>
+    </row>
+    <row r="1630" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1630">
+        <v>518</v>
+      </c>
+      <c r="B1630" t="s">
+        <v>3041</v>
+      </c>
+    </row>
+    <row r="1631" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1631">
+        <v>518</v>
+      </c>
+      <c r="B1631" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="1632" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1632">
+        <v>519</v>
+      </c>
+      <c r="B1632" t="s">
+        <v>2386</v>
+      </c>
+    </row>
+    <row r="1633" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1633">
+        <v>519</v>
+      </c>
+      <c r="B1633" t="s">
+        <v>3042</v>
+      </c>
+    </row>
+    <row r="1634" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1634">
+        <v>519</v>
+      </c>
+      <c r="B1634" t="s">
+        <v>3043</v>
+      </c>
+    </row>
+    <row r="1635" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1635">
+        <v>519</v>
+      </c>
+      <c r="B1635" t="s">
+        <v>3044</v>
+      </c>
+    </row>
+    <row r="1636" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1636">
+        <v>519</v>
+      </c>
+      <c r="B1636" t="s">
+        <v>3045</v>
+      </c>
+    </row>
+    <row r="1637" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1637">
+        <v>520</v>
+      </c>
+      <c r="B1637" t="s">
+        <v>2387</v>
+      </c>
+    </row>
+    <row r="1640" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1640">
+        <v>521</v>
+      </c>
+      <c r="B1640" t="s">
+        <v>2388</v>
+      </c>
+    </row>
+    <row r="1641" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1641">
+        <v>521</v>
+      </c>
+      <c r="B1641" t="s">
+        <v>3046</v>
+      </c>
+    </row>
+    <row r="1643" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1643">
+        <v>522</v>
+      </c>
+      <c r="B1643" t="s">
+        <v>2389</v>
+      </c>
+    </row>
+    <row r="1644" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1644">
+        <v>522</v>
+      </c>
+      <c r="B1644" t="s">
+        <v>3047</v>
+      </c>
+    </row>
+    <row r="1645" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1645">
+        <v>522</v>
+      </c>
+      <c r="B1645" t="s">
+        <v>3048</v>
+      </c>
+    </row>
+    <row r="1648" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1648">
+        <v>523</v>
+      </c>
+      <c r="B1648" t="s">
+        <v>2390</v>
+      </c>
+    </row>
+    <row r="1649" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1649">
+        <v>523</v>
+      </c>
+      <c r="B1649" t="s">
+        <v>3049</v>
+      </c>
+    </row>
+    <row r="1650" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1650">
+        <v>523</v>
+      </c>
+      <c r="B1650" t="s">
+        <v>3050</v>
+      </c>
+    </row>
+    <row r="1651" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1651">
+        <v>524</v>
+      </c>
+      <c r="B1651" t="s">
+        <v>2391</v>
+      </c>
+    </row>
+    <row r="1652" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1652">
+        <v>524</v>
+      </c>
+      <c r="B1652" t="s">
+        <v>3051</v>
+      </c>
+    </row>
+    <row r="1653" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1653">
+        <v>524</v>
+      </c>
+      <c r="B1653" t="s">
+        <v>3052</v>
+      </c>
+    </row>
+    <row r="1654" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1654">
+        <v>525</v>
+      </c>
+      <c r="B1654" t="s">
+        <v>2392</v>
+      </c>
+    </row>
+    <row r="1655" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1655">
+        <v>525</v>
+      </c>
+      <c r="B1655" t="s">
+        <v>3053</v>
+      </c>
+    </row>
+    <row r="1656" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1656">
+        <v>525</v>
+      </c>
+      <c r="B1656" t="s">
+        <v>3054</v>
+      </c>
+    </row>
+    <row r="1657" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1657">
+        <v>526</v>
+      </c>
+      <c r="B1657" t="s">
+        <v>2393</v>
+      </c>
+    </row>
+    <row r="1658" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1658">
+        <v>526</v>
+      </c>
+      <c r="B1658" t="s">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="1659" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1659">
+        <v>526</v>
+      </c>
+      <c r="B1659" t="s">
+        <v>3055</v>
+      </c>
+    </row>
+    <row r="1660" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1660">
+        <v>526</v>
+      </c>
+      <c r="B1660" t="s">
+        <v>3056</v>
+      </c>
+    </row>
+    <row r="1661" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1661">
+        <v>526</v>
+      </c>
+      <c r="B1661" t="s">
+        <v>3057</v>
+      </c>
+    </row>
+    <row r="1662" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1662">
+        <v>526</v>
+      </c>
+      <c r="B1662" t="s">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="1663" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1663">
+        <v>526</v>
+      </c>
+      <c r="B1663" t="s">
+        <v>2559</v>
+      </c>
+    </row>
+    <row r="1664" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1664">
+        <v>527</v>
+      </c>
+      <c r="B1664" t="s">
+        <v>2394</v>
+      </c>
+    </row>
+    <row r="1665" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1665">
+        <v>527</v>
+      </c>
+      <c r="B1665" t="s">
+        <v>1714</v>
+      </c>
+    </row>
+    <row r="1666" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1666">
+        <v>527</v>
+      </c>
+      <c r="B1666" t="s">
+        <v>3058</v>
+      </c>
+    </row>
+    <row r="1667" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1667">
+        <v>527</v>
+      </c>
+      <c r="B1667" t="s">
+        <v>2912</v>
+      </c>
+    </row>
+    <row r="1668" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1668">
+        <v>527</v>
+      </c>
+      <c r="B1668" t="s">
+        <v>1714</v>
+      </c>
+    </row>
+    <row r="1669" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1669">
         <v>528</v>
       </c>
-      <c r="B1611" t="s">
+      <c r="B1669" t="s">
         <v>2395</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B1611">
-    <sortCondition ref="A2:A1611"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B1671">
+    <sortCondition ref="A2:A1671"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>